<commit_message>
added age range graphs
</commit_message>
<xml_diff>
--- a/data/ireland_hospital_c19_stats.xlsx
+++ b/data/ireland_hospital_c19_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drelihan\OneDrive - Intel Corporation\Documents\covid19_analysis\ireland_covid19_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:40009_{DC5FC63E-D001-4253-A6A4-1C059D008374}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{24A90094-D1D9-4CA5-8998-AEA1BA74BA9A}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:40009_{DC5FC63E-D001-4253-A6A4-1C059D008374}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{18A4FFA5-FDE5-46EC-9E50-46511DE88285}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>date</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>available_icu_beds</t>
+  </si>
+  <si>
+    <t>c19_ventilated_cases</t>
   </si>
 </sst>
 </file>
@@ -881,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -893,9 +896,10 @@
     <col min="2" max="2" width="20.5546875" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="20.5546875" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -908,8 +912,11 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43934</v>
       </c>
@@ -922,8 +929,11 @@
       <c r="D2">
         <v>135</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43935</v>
       </c>
@@ -936,8 +946,11 @@
       <c r="D3">
         <v>133</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>43936</v>
       </c>
@@ -950,8 +963,11 @@
       <c r="D4">
         <v>127</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>43937</v>
       </c>
@@ -964,8 +980,11 @@
       <c r="D5">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43938</v>
       </c>
@@ -978,8 +997,11 @@
       <c r="D6">
         <v>126</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>43939</v>
       </c>
@@ -992,8 +1014,11 @@
       <c r="D7">
         <v>132</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>43940</v>
       </c>
@@ -1006,8 +1031,11 @@
       <c r="D8">
         <v>142</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>43941</v>
       </c>
@@ -1020,8 +1048,11 @@
       <c r="D9">
         <v>140</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>43942</v>
       </c>
@@ -1034,8 +1065,11 @@
       <c r="D10">
         <v>133</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>43943</v>
       </c>
@@ -1048,8 +1082,11 @@
       <c r="D11">
         <v>140</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>43944</v>
       </c>
@@ -1062,8 +1099,11 @@
       <c r="D12">
         <v>142</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>43945</v>
       </c>
@@ -1076,8 +1116,11 @@
       <c r="D13">
         <v>143</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>43946</v>
       </c>
@@ -1090,8 +1133,11 @@
       <c r="D14">
         <v>139</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>43947</v>
       </c>
@@ -1104,8 +1150,11 @@
       <c r="D15">
         <v>153</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>43948</v>
       </c>
@@ -1118,8 +1167,11 @@
       <c r="D16">
         <v>164</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>43949</v>
       </c>
@@ -1132,8 +1184,11 @@
       <c r="D17">
         <v>151</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>43950</v>
       </c>
@@ -1146,8 +1201,11 @@
       <c r="D18">
         <v>141</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>43951</v>
       </c>
@@ -1160,8 +1218,11 @@
       <c r="D19">
         <v>146</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>43952</v>
       </c>
@@ -1174,8 +1235,11 @@
       <c r="D20">
         <v>134</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>43953</v>
       </c>
@@ -1188,8 +1252,11 @@
       <c r="D21">
         <v>131</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43954</v>
       </c>
@@ -1202,13 +1269,28 @@
       <c r="D22">
         <v>143</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>43955</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>91</v>
+      </c>
+      <c r="C23" s="2">
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>132</v>
+      </c>
+      <c r="E23">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
@@ -1220,21 +1302,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006CA7C97186F1BB408A6F387D684A3BB6" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="58c7cd5724ce370d4d73babe3356d4a9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="04591d74-042e-4909-9ae6-bc115388d8f2" xmlns:ns4="514868b4-9db6-4edd-a163-6c6915c701a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="257ff94f7eb6a2de2f3f859f9e8efae4" ns3:_="" ns4:_="">
     <xsd:import namespace="04591d74-042e-4909-9ae6-bc115388d8f2"/>
@@ -1457,32 +1524,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40BE587D-E57A-4527-8E83-4C5AE2686BCA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="514868b4-9db6-4edd-a163-6c6915c701a5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="04591d74-042e-4909-9ae6-bc115388d8f2"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBCD0DD-E5BF-4854-A2AA-8E63557D0656}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E480AC8-B063-456D-AB59-C66FDDCF5808}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1499,4 +1556,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBCD0DD-E5BF-4854-A2AA-8E63557D0656}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40BE587D-E57A-4527-8E83-4C5AE2686BCA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="04591d74-042e-4909-9ae6-bc115388d8f2"/>
+    <ds:schemaRef ds:uri="514868b4-9db6-4edd-a163-6c6915c701a5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update for 5th of May
</commit_message>
<xml_diff>
--- a/data/ireland_hospital_c19_stats.xlsx
+++ b/data/ireland_hospital_c19_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drelihan\OneDrive - Intel Corporation\Documents\covid19_analysis\ireland_covid19_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:40009_{DC5FC63E-D001-4253-A6A4-1C059D008374}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{18A4FFA5-FDE5-46EC-9E50-46511DE88285}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="13_ncr:40009_{DC5FC63E-D001-4253-A6A4-1C059D008374}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{A34042F3-E768-4D0E-8596-3BEA1AA36D67}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">		</t>
   </si>
   <si>
     <t>c19_icu_cases</t>
@@ -887,7 +884,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -904,16 +901,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1291,8 +1288,20 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>1</v>
+      <c r="A24" s="1">
+        <v>43956</v>
+      </c>
+      <c r="B24">
+        <v>90</v>
+      </c>
+      <c r="C24" s="2">
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <v>145</v>
+      </c>
+      <c r="E24">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1302,6 +1311,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006CA7C97186F1BB408A6F387D684A3BB6" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="58c7cd5724ce370d4d73babe3356d4a9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="04591d74-042e-4909-9ae6-bc115388d8f2" xmlns:ns4="514868b4-9db6-4edd-a163-6c6915c701a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="257ff94f7eb6a2de2f3f859f9e8efae4" ns3:_="" ns4:_="">
     <xsd:import namespace="04591d74-042e-4909-9ae6-bc115388d8f2"/>
@@ -1524,15 +1542,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1540,6 +1549,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBCD0DD-E5BF-4854-A2AA-8E63557D0656}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E480AC8-B063-456D-AB59-C66FDDCF5808}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1558,26 +1575,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBCD0DD-E5BF-4854-A2AA-8E63557D0656}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40BE587D-E57A-4527-8E83-4C5AE2686BCA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="04591d74-042e-4909-9ae6-bc115388d8f2"/>
-    <ds:schemaRef ds:uri="514868b4-9db6-4edd-a163-6c6915c701a5"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="04591d74-042e-4909-9ae6-bc115388d8f2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="514868b4-9db6-4edd-a163-6c6915c701a5"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
6th of may updates
</commit_message>
<xml_diff>
--- a/data/ireland_hospital_c19_stats.xlsx
+++ b/data/ireland_hospital_c19_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drelihan\OneDrive - Intel Corporation\Documents\covid19_analysis\ireland_covid19_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="13_ncr:40009_{DC5FC63E-D001-4253-A6A4-1C059D008374}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{A34042F3-E768-4D0E-8596-3BEA1AA36D67}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86ADC6C0-CB13-4168-9238-35FC08CAA574}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -881,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1304,6 +1304,23 @@
         <v>53</v>
       </c>
     </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>43957</v>
+      </c>
+      <c r="B25">
+        <v>82</v>
+      </c>
+      <c r="C25" s="2">
+        <v>37</v>
+      </c>
+      <c r="D25">
+        <v>144</v>
+      </c>
+      <c r="E25">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1311,12 +1328,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1543,15 +1557,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBCD0DD-E5BF-4854-A2AA-8E63557D0656}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40BE587D-E57A-4527-8E83-4C5AE2686BCA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="04591d74-042e-4909-9ae6-bc115388d8f2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="514868b4-9db6-4edd-a163-6c6915c701a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1576,18 +1602,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40BE587D-E57A-4527-8E83-4C5AE2686BCA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBCD0DD-E5BF-4854-A2AA-8E63557D0656}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="04591d74-042e-4909-9ae6-bc115388d8f2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="514868b4-9db6-4edd-a163-6c6915c701a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
new data and refactoring
</commit_message>
<xml_diff>
--- a/data/ireland_hospital_c19_stats.xlsx
+++ b/data/ireland_hospital_c19_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drelihan\OneDrive - Intel Corporation\Documents\covid19_analysis\ireland_covid19_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="6_{75D2665C-C7CB-42C6-81CB-292544B512C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{1E67C89F-E5AC-499B-BD29-E6F24E5058CD}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="6_{75D2665C-C7CB-42C6-81CB-292544B512C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{7FDF6141-2533-4877-8305-1DB1BE9B7D2A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -881,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1457,6 +1457,125 @@
         <v>44</v>
       </c>
     </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>43966</v>
+      </c>
+      <c r="B34">
+        <v>56</v>
+      </c>
+      <c r="C34" s="2">
+        <v>16</v>
+      </c>
+      <c r="D34">
+        <v>155</v>
+      </c>
+      <c r="E34">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>43967</v>
+      </c>
+      <c r="B35">
+        <v>54</v>
+      </c>
+      <c r="C35" s="2">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>151</v>
+      </c>
+      <c r="E35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>43968</v>
+      </c>
+      <c r="B36">
+        <v>51</v>
+      </c>
+      <c r="C36" s="2">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>138</v>
+      </c>
+      <c r="E36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>43969</v>
+      </c>
+      <c r="B37">
+        <v>55</v>
+      </c>
+      <c r="C37" s="2">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>141</v>
+      </c>
+      <c r="E37">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>43970</v>
+      </c>
+      <c r="B38">
+        <v>54</v>
+      </c>
+      <c r="C38" s="2">
+        <v>16</v>
+      </c>
+      <c r="D38">
+        <v>132</v>
+      </c>
+      <c r="E38">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>43971</v>
+      </c>
+      <c r="B39">
+        <v>49</v>
+      </c>
+      <c r="C39" s="2">
+        <v>11</v>
+      </c>
+      <c r="D39">
+        <v>126</v>
+      </c>
+      <c r="E39">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>43972</v>
+      </c>
+      <c r="B40">
+        <v>52</v>
+      </c>
+      <c r="C40" s="2">
+        <v>12</v>
+      </c>
+      <c r="D40">
+        <v>109</v>
+      </c>
+      <c r="E40">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1464,12 +1583,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1696,15 +1812,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBCD0DD-E5BF-4854-A2AA-8E63557D0656}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40BE587D-E57A-4527-8E83-4C5AE2686BCA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="514868b4-9db6-4edd-a163-6c6915c701a5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="04591d74-042e-4909-9ae6-bc115388d8f2"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1729,18 +1857,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40BE587D-E57A-4527-8E83-4C5AE2686BCA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBCD0DD-E5BF-4854-A2AA-8E63557D0656}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="514868b4-9db6-4edd-a163-6c6915c701a5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="04591d74-042e-4909-9ae6-bc115388d8f2"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
reorder and update cases
</commit_message>
<xml_diff>
--- a/data/ireland_hospital_c19_stats.xlsx
+++ b/data/ireland_hospital_c19_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drelihan\OneDrive - Intel Corporation\Documents\ireland_covid19_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="247" documentId="6_{C79A1026-B183-4477-861F-E8251FC0E225}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6C5C160E-6E52-4F1D-83B7-A57068ED526A}"/>
+  <xr:revisionPtr revIDLastSave="251" documentId="6_{C79A1026-B183-4477-861F-E8251FC0E225}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A41FE15-62F6-4407-9B4D-9215A699F396}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -875,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D116"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2512,6 +2512,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>44049</v>
+      </c>
+      <c r="B117">
+        <v>5</v>
+      </c>
+      <c r="C117">
+        <v>34</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2519,6 +2533,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006CA7C97186F1BB408A6F387D684A3BB6" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="58c7cd5724ce370d4d73babe3356d4a9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="04591d74-042e-4909-9ae6-bc115388d8f2" xmlns:ns4="514868b4-9db6-4edd-a163-6c6915c701a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="257ff94f7eb6a2de2f3f859f9e8efae4" ns3:_="" ns4:_="">
     <xsd:import namespace="04591d74-042e-4909-9ae6-bc115388d8f2"/>
@@ -2741,22 +2770,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40BE587D-E57A-4527-8E83-4C5AE2686BCA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="04591d74-042e-4909-9ae6-bc115388d8f2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="514868b4-9db6-4edd-a163-6c6915c701a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBCD0DD-E5BF-4854-A2AA-8E63557D0656}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E480AC8-B063-456D-AB59-C66FDDCF5808}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2773,29 +2812,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBCD0DD-E5BF-4854-A2AA-8E63557D0656}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40BE587D-E57A-4527-8E83-4C5AE2686BCA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="04591d74-042e-4909-9ae6-bc115388d8f2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="514868b4-9db6-4edd-a163-6c6915c701a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>